<commit_message>
Added robot framework test files and python utilities
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>zaff</t>
+  </si>
+  <si>
+    <t>aydan</t>
+  </si>
+  <si>
+    <t>jk</t>
   </si>
 </sst>
 </file>
@@ -382,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -426,6 +432,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>

</xml_diff>